<commit_message>
1.查看qa2016-1-10 194515 2.补充qa22016-1-11 222234 3.更新周计划2016 4.补2016.1.13学习计划每日进展
</commit_message>
<xml_diff>
--- a/周计划2016.xlsx
+++ b/周计划2016.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
   <si>
     <t>星期一</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -690,34 +690,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Mon</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tue</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Wed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Thur</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fri</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sat</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sun</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -904,7 +876,7 @@
         <scheme val="minor"/>
       </rPr>
       <t>整合高斯、余弦功能；衰减控制联调
-      8.</t>
+      8.上位机增加烧写功能；ARM增加烧写FLASH功能</t>
     </r>
     <r>
       <rPr>
@@ -915,7 +887,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">上位机增加烧写功能；ARM增加烧写FLASH功能
+      <t xml:space="preserve">
      </t>
     </r>
     <r>
@@ -943,10 +915,46 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1.GR6017上位机衰减控制逻辑
+    <t>星期一</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.GR6017上位机衰减控制逻辑
 2.GR6017 ARM Flash 读写；衰减发送
 3.解决Jlink Or STLink 仿真器连接失败的问题
-4.58个英语单词</t>
+4.58个英语单词
+5.《计算机网络自顶向下》 Cookies（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>初步阅读</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.79个英语单词：复习49，新增30
+2.天奥联调：
+    测试GR6017上位机及下位机新增的FLASH固化功能；
+    以及上位机的文件保存和下载功能</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1725,10 +1733,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1736,7 +1744,7 @@
     <col min="1" max="1" width="40.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="46.125" style="1" customWidth="1"/>
     <col min="3" max="3" width="22.75" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.625" style="1" customWidth="1"/>
     <col min="5" max="5" width="28.75" style="1" customWidth="1"/>
     <col min="6" max="6" width="15.5" style="1" customWidth="1"/>
     <col min="7" max="7" width="16.75" style="1" customWidth="1"/>
@@ -1744,33 +1752,34 @@
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="23" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="23" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>25</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="112.5" customHeight="1" x14ac:dyDescent="0.15">
+        <v>7</v>
+      </c>
+      <c r="I1" s="22"/>
+    </row>
+    <row r="2" spans="1:9" ht="132.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>22</v>
       </c>
@@ -1781,14 +1790,15 @@
         <v>24</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="8"/>
+        <v>28</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="G2" s="8"/>
       <c r="H2" s="6"/>
     </row>
-    <row r="3" spans="1:8" ht="54" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" ht="54" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>23</v>
       </c>
@@ -1800,9 +1810,9 @@
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:8" ht="216" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" ht="216" x14ac:dyDescent="0.15">
       <c r="A4" s="19" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -1812,7 +1822,7 @@
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:8" ht="54" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" ht="54" x14ac:dyDescent="0.15">
       <c r="A5" s="9" t="s">
         <v>13</v>
       </c>
@@ -1824,7 +1834,7 @@
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
     </row>
-    <row r="6" spans="1:8" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A6" s="9" t="s">
         <v>14</v>
       </c>
@@ -1836,7 +1846,7 @@
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="20" t="s">
         <v>20</v>
       </c>
@@ -1848,7 +1858,7 @@
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="20" t="s">
         <v>17</v>
       </c>
@@ -1860,12 +1870,12 @@
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="5"/>
     </row>
   </sheetData>

</xml_diff>